<commit_message>
Reviewing CRS V1.0 (#8)
</commit_message>
<xml_diff>
--- a/Input Document/CRS/Review/PO_SB_CRS_WEB_Review.xlsx
+++ b/Input Document/CRS/Review/PO_SB_CRS_WEB_Review.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Graduation_Project\Web_SWProcess_Documents\input Documant\cr\Review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Repos\SB\Web_SWProcess_Documents\Input Document\CRS\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DEC5548-4165-40D1-8AF8-99FC541CB1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E5C471-D9ED-4DC7-90F7-F637D835BE5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ورقة1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="51">
   <si>
     <t>Entry Date</t>
   </si>
@@ -47,7 +46,133 @@
     <t>Proposed Solution</t>
   </si>
   <si>
-    <t>CR_REV_ID</t>
+    <t>CRS_REV_ID</t>
+  </si>
+  <si>
+    <t>CRS_REV_001</t>
+  </si>
+  <si>
+    <t>Ammar Yasser</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
+  <si>
+    <t>3//Project Description/PO_SB_CRS_003-V1.0</t>
+  </si>
+  <si>
+    <t>all oauth providers are listed together</t>
+  </si>
+  <si>
+    <t>every oauth provider shall be listed on it's own requirement</t>
+  </si>
+  <si>
+    <t>CRS_REV_002</t>
+  </si>
+  <si>
+    <t>"displays informations" is a general word that can be described in more details</t>
+  </si>
+  <si>
+    <t>shall list product features , reviews</t>
+  </si>
+  <si>
+    <t>CRS_REV_003</t>
+  </si>
+  <si>
+    <t>the sentence implies that the payment process happens in the landing page</t>
+  </si>
+  <si>
+    <t>4//Project Description/PO_SB_CRS_005-V1.0</t>
+  </si>
+  <si>
+    <t>4//Project Description/PO_SB_CRS_006-V1.0</t>
+  </si>
+  <si>
+    <t>description shall be "a buy now button shall redirects the user to the payment page"</t>
+  </si>
+  <si>
+    <t>CRS_REV_004</t>
+  </si>
+  <si>
+    <t>4//Project Description/PO_SB_CRS_008-V1.0 &amp; PO_SB_CRS_009-V1.0</t>
+  </si>
+  <si>
+    <t>payment senario isn't described in details</t>
+  </si>
+  <si>
+    <t>senario shall be described more in details , like listing payment options , entry of address , summary and confirmation of the order</t>
+  </si>
+  <si>
+    <t>CRS_REV_005</t>
+  </si>
+  <si>
+    <t>4//Project Description/PO_SB_CRS_0010-V1.0</t>
+  </si>
+  <si>
+    <t>order traking status is not listed</t>
+  </si>
+  <si>
+    <t>order traking status shall be listed like = "out for delivery , delivered , not configured"</t>
+  </si>
+  <si>
+    <t>CRS_REV_006</t>
+  </si>
+  <si>
+    <t>4//Project Description/PO_SB_CRS_0011-V1.0</t>
+  </si>
+  <si>
+    <t>description is not clear on how the customer shall send the feedback</t>
+  </si>
+  <si>
+    <t>description shall illustrate in details how the user will send the feedback for example it could be through a form , mail , chat</t>
+  </si>
+  <si>
+    <t>CRS_REV_007</t>
+  </si>
+  <si>
+    <t>5//Project Description/PO_SB_CRS_0012-V1.0</t>
+  </si>
+  <si>
+    <t>different rules are listed together</t>
+  </si>
+  <si>
+    <t>every rule shall be listed on it's own requirement</t>
+  </si>
+  <si>
+    <t>CRS_REV_008</t>
+  </si>
+  <si>
+    <t>5//Project Description/PO_SB_CRS_0014-V1.0 to 0017</t>
+  </si>
+  <si>
+    <t>permission of each type of dashboard user isn't disscussed in details</t>
+  </si>
+  <si>
+    <t>permission of each type of dashboard user shall be illustrated in details like "super admin can do 1 , 2 , 3" **EACH ONE IN IT'S OWN REQ**</t>
+  </si>
+  <si>
+    <t>CRS_REV_009</t>
+  </si>
+  <si>
+    <t>CRS_REV_010</t>
+  </si>
+  <si>
+    <t>5//Project Description/PO_SB_CRS_0018-V1.0</t>
+  </si>
+  <si>
+    <t>description is not discriptive on how the admin shall use the account</t>
+  </si>
+  <si>
+    <t>description shall be "dashboard admins can login to the dashboard using email and password" SIDE-NOTE:"Can reset password?"</t>
+  </si>
+  <si>
+    <t>5//Project Description/PO_SB_CRS_0019-V1.0 to 0022</t>
+  </si>
+  <si>
+    <t>KINDLY take your time to rewrite the mentioned requirements</t>
+  </si>
+  <si>
+    <t>Description of the mentioned requirements is not illustrated in details</t>
   </si>
 </sst>
 </file>
@@ -57,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -81,6 +206,10 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -137,15 +266,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -159,9 +282,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="عادي" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF57BB8A"/>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF57BB8A"/>
+          <bgColor rgb="FF57BB8A"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -399,23 +568,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="32.28515625" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
-    <col min="6" max="7" width="44.5703125" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="5" max="5" width="42.5546875" customWidth="1"/>
+    <col min="6" max="7" width="44.5546875" customWidth="1"/>
+    <col min="8" max="8" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -441,132 +610,473 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="4">
+        <v>44876</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="14.4" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="A2:H9 A10:D25">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>$H2 = "Closed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:H9">
-    <cfRule type="expression" dxfId="0" priority="4">
+  <conditionalFormatting sqref="A2:H9 A10:D25">
+    <cfRule type="expression" dxfId="4" priority="8">
       <formula>$H2= "Open"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F10:H10 E11:H25">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$H10 = "Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:H10 E11:H25">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$H10= "Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$H10 = "Closed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>$H10= "Open"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H9" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" prompt="Open" sqref="H2:H25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9B076B-6709-46BB-9DBF-3558C54B2CEA}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>